<commit_message>
Change basic_delivery and complex_delivery
</commit_message>
<xml_diff>
--- a/appGreece/config/tables/basic_delivery/forms/basic_delivery/basic_delivery.xlsx
+++ b/appGreece/config/tables/basic_delivery/forms/basic_delivery/basic_delivery.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RedCrossWorkspace\app-designer\appGreece\config\tables\basic_delivery\forms\basic_delivery\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3158" yWindow="623" windowWidth="44003" windowHeight="23198" tabRatio="362"/>
+    <workbookView xWindow="3160" yWindow="620" windowWidth="44000" windowHeight="23200" tabRatio="362" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="5" r:id="rId1"/>
@@ -19,14 +14,15 @@
     <sheet name="choices" sheetId="4" r:id="rId5"/>
     <sheet name="calculates" sheetId="6" r:id="rId6"/>
     <sheet name="properties" sheetId="7" r:id="rId7"/>
+    <sheet name="initial" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -36,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
   <si>
     <t>type</t>
   </si>
@@ -240,12 +236,21 @@
   </si>
   <si>
     <t>isDelivered</t>
+  </si>
+  <si>
+    <t>display.text</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>do section survey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -401,7 +406,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -447,6 +452,9 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -789,7 +797,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -799,25 +807,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.6875" customWidth="1"/>
-    <col min="2" max="2" width="53.8125" customWidth="1"/>
-    <col min="3" max="3" width="30.3125" customWidth="1"/>
-    <col min="4" max="4" width="15.1875" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="53.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
     <col min="5" max="5" width="30.5" customWidth="1"/>
     <col min="6" max="6" width="88.5" customWidth="1"/>
     <col min="7" max="7" width="50" customWidth="1"/>
-    <col min="8" max="8" width="26.3125" customWidth="1"/>
-    <col min="9" max="9" width="44.1875" customWidth="1"/>
-    <col min="10" max="10" width="48.1875" customWidth="1"/>
+    <col min="8" max="8" width="26.33203125" customWidth="1"/>
+    <col min="9" max="9" width="44.1640625" customWidth="1"/>
+    <col min="10" max="10" width="48.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:21" ht="23">
       <c r="A1" s="6" t="s">
         <v>33</v>
       </c>
@@ -852,7 +860,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:21" ht="23">
       <c r="A2" s="9" t="s">
         <v>56</v>
       </c>
@@ -864,7 +872,7 @@
       <c r="G2" s="34"/>
       <c r="H2" s="35"/>
     </row>
-    <row r="3" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:21" ht="23">
       <c r="A3" s="9"/>
       <c r="B3" s="17"/>
       <c r="C3" s="18" t="s">
@@ -893,7 +901,7 @@
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
     </row>
-    <row r="4" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:21" ht="23">
       <c r="A4" s="22"/>
       <c r="B4" s="23"/>
       <c r="C4" s="24"/>
@@ -922,7 +930,7 @@
       <c r="T4" s="11"/>
       <c r="U4" s="11"/>
     </row>
-    <row r="5" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:21" ht="23">
       <c r="A5" s="22" t="s">
         <v>57</v>
       </c>
@@ -947,7 +955,7 @@
       <c r="T5" s="11"/>
       <c r="U5" s="11"/>
     </row>
-    <row r="6" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:21" ht="23">
       <c r="A6" s="22"/>
       <c r="B6" s="23"/>
       <c r="C6" s="24" t="s">
@@ -976,7 +984,7 @@
       <c r="T6" s="11"/>
       <c r="U6" s="11"/>
     </row>
-    <row r="7" spans="1:21" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:21" ht="23">
       <c r="A7" s="22"/>
       <c r="B7" s="23"/>
       <c r="C7" s="24"/>
@@ -1018,14 +1026,14 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="18.3125" customWidth="1"/>
-    <col min="2" max="2" width="34.3125" customWidth="1"/>
-    <col min="3" max="3" width="34.6875" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1"/>
+    <col min="3" max="3" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:2" ht="23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1033,7 +1041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:2" ht="23">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1041,7 +1049,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:2" ht="23">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1049,7 +1057,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:2" ht="23">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1057,7 +1065,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:2" ht="23">
       <c r="A5" s="3" t="s">
         <v>65</v>
       </c>
@@ -1084,14 +1092,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.1875" customWidth="1"/>
-    <col min="2" max="2" width="30.8125" customWidth="1"/>
-    <col min="3" max="3" width="26.8125" customWidth="1"/>
+    <col min="1" max="1" width="28.1640625" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:3" ht="23">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -1102,7 +1110,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:3" ht="23">
       <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
@@ -1111,7 +1119,7 @@
       </c>
       <c r="C2" s="10"/>
     </row>
-    <row r="3" spans="1:3" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:3" ht="23">
       <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
@@ -1120,7 +1128,7 @@
       </c>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:3" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:3" ht="23">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
@@ -1129,7 +1137,7 @@
       </c>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:3" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:3" ht="23">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -1138,7 +1146,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="23.25" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:3" ht="23">
       <c r="A6" s="8" t="s">
         <v>17</v>
       </c>
@@ -1166,14 +1174,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.3125" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="17.1875" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1181,7 +1189,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1189,7 +1197,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1197,7 +1205,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1205,7 +1213,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1213,7 +1221,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1240,14 +1248,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.3125" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1258,7 +1266,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1269,7 +1277,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1299,13 +1307,13 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.6875" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="128.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1313,10 +1321,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2">
       <c r="B2" s="27"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:2">
       <c r="B3" s="27"/>
     </row>
   </sheetData>
@@ -1338,16 +1346,16 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.1875" customWidth="1"/>
-    <col min="2" max="2" width="15.6875" customWidth="1"/>
-    <col min="3" max="3" width="29.8125" customWidth="1"/>
-    <col min="4" max="4" width="21.6875" customWidth="1"/>
-    <col min="5" max="5" width="19.3125" customWidth="1"/>
+    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="29.83203125" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5">
       <c r="A1" s="11" t="s">
         <v>44</v>
       </c>
@@ -1364,7 +1372,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5">
       <c r="A2" s="11" t="s">
         <v>47</v>
       </c>
@@ -1381,7 +1389,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1398,7 +1406,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1424,4 +1432,51 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
skip finalize on basic_delivery
</commit_message>
<xml_diff>
--- a/appGreece/config/tables/basic_delivery/forms/basic_delivery/basic_delivery.xlsx
+++ b/appGreece/config/tables/basic_delivery/forms/basic_delivery/basic_delivery.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/redcross/app-designer/appGreece/config/tables/basic_delivery/forms/basic_delivery/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="3160" yWindow="620" windowWidth="44000" windowHeight="23200" tabRatio="362" activeTab="7"/>
   </bookViews>
@@ -18,11 +23,11 @@
   </sheets>
   <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="330"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -32,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73">
   <si>
     <t>type</t>
   </si>
@@ -245,6 +250,12 @@
   </si>
   <si>
     <t>do section survey</t>
+  </si>
+  <si>
+    <t>goto _finalize</t>
+  </si>
+  <si>
+    <t>skips the finalize screen where the user chooses to save as incomplete or finalized and instead saves as finalized</t>
   </si>
 </sst>
 </file>
@@ -797,7 +808,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -811,7 +822,7 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="53.83203125" customWidth="1"/>
@@ -825,7 +836,7 @@
     <col min="10" max="10" width="48.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="23">
+    <row r="1" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>33</v>
       </c>
@@ -860,7 +871,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="23">
+    <row r="2" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>56</v>
       </c>
@@ -872,7 +883,7 @@
       <c r="G2" s="34"/>
       <c r="H2" s="35"/>
     </row>
-    <row r="3" spans="1:21" ht="23">
+    <row r="3" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
       <c r="B3" s="17"/>
       <c r="C3" s="18" t="s">
@@ -901,7 +912,7 @@
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
     </row>
-    <row r="4" spans="1:21" ht="23">
+    <row r="4" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="22"/>
       <c r="B4" s="23"/>
       <c r="C4" s="24"/>
@@ -930,7 +941,7 @@
       <c r="T4" s="11"/>
       <c r="U4" s="11"/>
     </row>
-    <row r="5" spans="1:21" ht="23">
+    <row r="5" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="22" t="s">
         <v>57</v>
       </c>
@@ -955,7 +966,7 @@
       <c r="T5" s="11"/>
       <c r="U5" s="11"/>
     </row>
-    <row r="6" spans="1:21" ht="23">
+    <row r="6" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="22"/>
       <c r="B6" s="23"/>
       <c r="C6" s="24" t="s">
@@ -984,7 +995,7 @@
       <c r="T6" s="11"/>
       <c r="U6" s="11"/>
     </row>
-    <row r="7" spans="1:21" ht="23">
+    <row r="7" spans="1:21" ht="24" x14ac:dyDescent="0.3">
       <c r="A7" s="22"/>
       <c r="B7" s="23"/>
       <c r="C7" s="24"/>
@@ -1010,11 +1021,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1026,14 +1032,14 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="34.33203125" customWidth="1"/>
     <col min="3" max="3" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23">
+    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1041,7 +1047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="23">
+    <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1049,7 +1055,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="23">
+    <row r="3" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1057,7 +1063,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="23">
+    <row r="4" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1065,7 +1071,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="23">
+    <row r="5" spans="1:2" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>65</v>
       </c>
@@ -1076,11 +1082,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1092,14 +1093,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28.1640625" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" customWidth="1"/>
     <col min="3" max="3" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="23">
+    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -1110,7 +1111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="23">
+    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
@@ -1119,7 +1120,7 @@
       </c>
       <c r="C2" s="10"/>
     </row>
-    <row r="3" spans="1:3" ht="23">
+    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
@@ -1128,7 +1129,7 @@
       </c>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:3" ht="23">
+    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
@@ -1137,7 +1138,7 @@
       </c>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:3" ht="23">
+    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -1146,7 +1147,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="23">
+    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>17</v>
       </c>
@@ -1158,11 +1159,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1174,14 +1170,14 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1189,7 +1185,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1197,7 +1193,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1205,7 +1201,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1213,7 +1209,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1221,7 +1217,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1232,11 +1228,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1248,14 +1239,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1266,7 +1257,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1277,7 +1268,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -1291,11 +1282,6 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1307,13 +1293,13 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="128.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -1321,20 +1307,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B2" s="27"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B3" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -1346,7 +1327,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
@@ -1355,7 +1336,7 @@
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>44</v>
       </c>
@@ -1372,7 +1353,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>47</v>
       </c>
@@ -1389,7 +1370,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>51</v>
       </c>
@@ -1406,7 +1387,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>51</v>
       </c>
@@ -1426,23 +1407,18 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
@@ -1450,7 +1426,7 @@
     <col min="4" max="4" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
         <v>33</v>
       </c>
@@ -1464,19 +1440,24 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
         <v>70</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
     </row>
+    <row r="3" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="A3" s="37" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
naming and assignment fixes basic_delivery
</commit_message>
<xml_diff>
--- a/appGreece/config/tables/basic_delivery/forms/basic_delivery/basic_delivery.xlsx
+++ b/appGreece/config/tables/basic_delivery/forms/basic_delivery/basic_delivery.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="620" windowWidth="44000" windowHeight="23200" tabRatio="362" activeTab="7"/>
+    <workbookView xWindow="3160" yWindow="620" windowWidth="44000" windowHeight="23200" tabRatio="362"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="properties" sheetId="7" r:id="rId7"/>
     <sheet name="initial" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="73">
   <si>
     <t>type</t>
   </si>
@@ -240,9 +240,6 @@
     <t>assign</t>
   </si>
   <si>
-    <t>isDelivered</t>
-  </si>
-  <si>
     <t>display.text</t>
   </si>
   <si>
@@ -256,6 +253,9 @@
   </si>
   <si>
     <t>skips the finalize screen where the user chooses to save as incomplete or finalized and instead saves as finalized</t>
+  </si>
+  <si>
+    <t>"TRUE"</t>
   </si>
 </sst>
 </file>
@@ -818,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -974,13 +974,13 @@
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="4" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="F6" s="30"/>
       <c r="G6" s="25"/>
       <c r="H6" s="26"/>
-      <c r="I6" s="11" t="b">
-        <v>1</v>
+      <c r="I6" s="11" t="s">
+        <v>72</v>
       </c>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
@@ -1414,7 +1414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -1434,27 +1434,27 @@
         <v>0</v>
       </c>
       <c r="C1" s="37" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="37" t="s">
         <v>68</v>
-      </c>
-      <c r="D1" s="37" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="37" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
     </row>
     <row r="3" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A3" s="37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
       <c r="D3" s="37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing names for delivery forms
</commit_message>
<xml_diff>
--- a/appGreece/config/tables/basic_delivery/forms/basic_delivery/basic_delivery.xlsx
+++ b/appGreece/config/tables/basic_delivery/forms/basic_delivery/basic_delivery.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ori/Documents/redcross/app-designer/appGreece/config/tables/basic_delivery/forms/basic_delivery/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="620" windowWidth="44000" windowHeight="23200" tabRatio="362"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="362" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="5" r:id="rId1"/>
@@ -21,13 +16,13 @@
     <sheet name="properties" sheetId="7" r:id="rId7"/>
     <sheet name="initial" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -37,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="73">
   <si>
     <t>type</t>
   </si>
@@ -126,9 +121,6 @@
     <t>yes_no</t>
   </si>
   <si>
-    <t>true</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -219,24 +211,9 @@
     <t>Basic Delivery</t>
   </si>
   <si>
-    <t>Distribute the Ice Skates</t>
-  </si>
-  <si>
-    <t>What size of skate?</t>
-  </si>
-  <si>
-    <t>Foot Size of Skate</t>
-  </si>
-  <si>
     <t>instruction</t>
   </si>
   <si>
-    <t>skatesize</t>
-  </si>
-  <si>
-    <t>decimal</t>
-  </si>
-  <si>
     <t>assign</t>
   </si>
   <si>
@@ -256,6 +233,24 @@
   </si>
   <si>
     <t>"TRUE"</t>
+  </si>
+  <si>
+    <t>Distribute the hygiene kit</t>
+  </si>
+  <si>
+    <t>Did the supplies last you the entire month?</t>
+  </si>
+  <si>
+    <t>supply</t>
+  </si>
+  <si>
+    <t>select_one</t>
+  </si>
+  <si>
+    <t>TRUE</t>
+  </si>
+  <si>
+    <t>FALSE</t>
   </si>
 </sst>
 </file>
@@ -412,8 +407,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -467,9 +466,13 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -808,7 +811,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -818,11 +821,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.6640625" customWidth="1"/>
     <col min="2" max="2" width="53.83203125" customWidth="1"/>
@@ -836,44 +839,44 @@
     <col min="10" max="10" width="48.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="23">
       <c r="A1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="H1" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="I1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>40</v>
       </c>
-      <c r="K1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:21" ht="23">
       <c r="A2" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="32"/>
@@ -883,18 +886,18 @@
       <c r="G2" s="34"/>
       <c r="H2" s="35"/>
     </row>
-    <row r="3" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="23">
       <c r="A3" s="9"/>
       <c r="B3" s="17"/>
       <c r="C3" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="21"/>
@@ -912,20 +915,22 @@
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
     </row>
-    <row r="4" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="23">
       <c r="A4" s="22"/>
       <c r="B4" s="23"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
+      <c r="C4" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>28</v>
+      </c>
       <c r="E4" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>62</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="G4" s="25"/>
       <c r="H4" s="26"/>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
@@ -941,9 +946,9 @@
       <c r="T4" s="11"/>
       <c r="U4" s="11"/>
     </row>
-    <row r="5" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="23">
       <c r="A5" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="24"/>
@@ -966,11 +971,11 @@
       <c r="T5" s="11"/>
       <c r="U5" s="11"/>
     </row>
-    <row r="6" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="23">
       <c r="A6" s="22"/>
       <c r="B6" s="23"/>
       <c r="C6" s="24" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D6" s="24"/>
       <c r="E6" s="4" t="s">
@@ -980,7 +985,7 @@
       <c r="G6" s="25"/>
       <c r="H6" s="26"/>
       <c r="I6" s="11" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J6" s="11"/>
       <c r="K6" s="11"/>
@@ -995,7 +1000,7 @@
       <c r="T6" s="11"/>
       <c r="U6" s="11"/>
     </row>
-    <row r="7" spans="1:21" ht="24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="23">
       <c r="A7" s="22"/>
       <c r="B7" s="23"/>
       <c r="C7" s="24"/>
@@ -1021,6 +1026,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1028,18 +1038,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
     <col min="2" max="2" width="34.33203125" customWidth="1"/>
     <col min="3" max="3" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="23">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1047,7 +1057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="23">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1055,7 +1065,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" ht="23">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1063,7 +1073,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="23">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1071,17 +1081,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" ht="23">
       <c r="A5" s="3" t="s">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1093,14 +1108,14 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="28.1640625" customWidth="1"/>
     <col min="2" max="2" width="30.83203125" customWidth="1"/>
     <col min="3" max="3" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="23">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -1111,16 +1126,16 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="23">
       <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="10"/>
     </row>
-    <row r="3" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="23">
       <c r="A3" s="8" t="s">
         <v>14</v>
       </c>
@@ -1129,25 +1144,25 @@
       </c>
       <c r="C3" s="10"/>
     </row>
-    <row r="4" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="23">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="10"/>
     </row>
-    <row r="5" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="23">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="24" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="23">
       <c r="A6" s="8" t="s">
         <v>17</v>
       </c>
@@ -1159,6 +1174,11 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1167,17 +1187,17 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="24.33203125" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -1185,7 +1205,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1193,7 +1213,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1201,7 +1221,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1209,7 +1229,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1217,7 +1237,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1228,6 +1248,11 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1236,17 +1261,17 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -1257,31 +1282,36 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>28</v>
       </c>
       <c r="B3" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" t="s">
         <v>31</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1293,29 +1323,34 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="128.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="B2" s="27"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2">
       <c r="B3" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1327,7 +1362,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.1640625" customWidth="1"/>
     <col min="2" max="2" width="15.6640625" customWidth="1"/>
@@ -1336,15 +1371,15 @@
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>46</v>
       </c>
       <c r="D1" s="11" t="s">
         <v>0</v>
@@ -1353,60 +1388,65 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>49</v>
       </c>
       <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="E2" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>51</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>52</v>
-      </c>
-      <c r="C3" t="s">
-        <v>53</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
         <v>51</v>
       </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1418,7 +1458,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
@@ -1426,38 +1466,43 @@
     <col min="4" max="4" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D1" s="37" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="37" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B2" s="37"/>
       <c r="C2" s="37"/>
     </row>
-    <row r="3" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="75">
       <c r="A3" s="37" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
       <c r="D3" s="37" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>